<commit_message>
Correcciones de validaciones en campos emailemp webemp
</commit_message>
<xml_diff>
--- a/docs/Correcciones revisión.xlsx
+++ b/docs/Correcciones revisión.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="134">
   <si>
     <t>N°</t>
   </si>
@@ -447,12 +447,15 @@
   <si>
     <t>coreción</t>
   </si>
+  <si>
+    <t>en el caso de que la fuente no pueda modificar el valor este caso solo aplica para la creacion del directorio base</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,8 +507,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,6 +530,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -528,17 +555,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -552,30 +577,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -585,22 +592,73 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -898,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H10"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,7 +1002,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -959,1522 +1017,1616 @@
       <c r="H3" s="21"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="24">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="25">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="18"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="13"/>
       <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="18"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="13"/>
       <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="18"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="13"/>
       <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="26">
         <v>3</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>16</v>
-      </c>
+      <c r="E11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="18"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="13"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="3" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="13"/>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>4</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>16</v>
+      <c r="E14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="36" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="13">
         <v>5</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="26" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="18"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="10" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="18"/>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="18"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="26"/>
     </row>
     <row r="19" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="10" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="18"/>
+      <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="18"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="18"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="26"/>
     </row>
     <row r="22" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="13">
         <v>6</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="12"/>
+      <c r="E22" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="10" t="s">
+      <c r="A23" s="13"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="12"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="12"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="10" t="s">
+      <c r="A25" s="13"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="12"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="A27" s="13">
         <v>7</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="12"/>
+      <c r="E27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="10" t="s">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="18"/>
-      <c r="F28" s="12"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="12"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="10" t="s">
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="12"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="12"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="12"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
+      <c r="A33" s="13">
         <v>8</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="12"/>
+      <c r="E33" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="12"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="10" t="s">
+      <c r="A35" s="13"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="12"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="13" t="s">
+      <c r="A36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="12"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="12"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="12"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="12"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A40" s="12">
+      <c r="A40" s="13">
         <v>9</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="12"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="12"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="10" t="s">
+      <c r="A42" s="13"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="18"/>
-      <c r="F42" s="12"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="12"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6" ht="84" x14ac:dyDescent="0.25">
-      <c r="A44" s="12">
+      <c r="A44" s="13">
         <v>10</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E44" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="12"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="12"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="14"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="12"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="10" t="s">
+      <c r="A47" s="13"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="18"/>
-      <c r="F47" s="12"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="12"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="12"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="12"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A51" s="12">
+      <c r="A51" s="13">
         <v>11</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E51" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" s="12"/>
+      <c r="E51" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="12"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="10" t="s">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E53" s="18"/>
-      <c r="F53" s="12"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="13" t="s">
+      <c r="A54" s="13"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="18"/>
-      <c r="F54" s="12"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="14"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="12"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="10" t="s">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E56" s="18"/>
-      <c r="F56" s="12"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="12"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="14"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="12"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="14"/>
     </row>
     <row r="59" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="12">
+      <c r="A59" s="13">
         <v>12</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D59" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F59" s="12"/>
+      <c r="E59" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="14"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="12"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="14"/>
     </row>
     <row r="61" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>13</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E61" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F61" s="11"/>
+      <c r="E61" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A62" s="12">
+      <c r="A62" s="13">
         <v>14</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E62" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F62" s="12"/>
+      <c r="E62" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="12"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="10" t="s">
+      <c r="A64" s="13"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E64" s="18"/>
-      <c r="F64" s="12"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="13" t="s">
+      <c r="A65" s="13"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E65" s="18"/>
-      <c r="F65" s="12"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="12"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="14"/>
     </row>
     <row r="67" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="10" t="s">
+      <c r="A67" s="13"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E67" s="18"/>
-      <c r="F67" s="12"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="14"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="10" t="s">
+      <c r="A68" s="13"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E68" s="18"/>
-      <c r="F68" s="12"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="14"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="10"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="12"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="14"/>
     </row>
     <row r="70" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="12">
+      <c r="A70" s="13">
         <v>15</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B70" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D70" s="14" t="s">
+      <c r="D70" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E70" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F70" s="12"/>
+      <c r="E70" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70" s="14"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="12"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="14"/>
     </row>
     <row r="72" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A72" s="12">
-        <v>16</v>
-      </c>
-      <c r="B72" s="12" t="s">
+      <c r="A72" s="13">
+        <v>16</v>
+      </c>
+      <c r="B72" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="D72" s="10" t="s">
+      <c r="D72" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E72" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F72" s="12"/>
+      <c r="E72" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F72" s="14"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="12"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="14"/>
     </row>
     <row r="74" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="10" t="s">
+      <c r="A74" s="13"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E74" s="18"/>
-      <c r="F74" s="12"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="14"/>
     </row>
     <row r="75" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="13" t="s">
+      <c r="A75" s="13"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E75" s="18"/>
-      <c r="F75" s="12"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="14"/>
     </row>
     <row r="76" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A76" s="12">
+      <c r="A76" s="13">
         <v>17</v>
       </c>
-      <c r="B76" s="12" t="s">
+      <c r="B76" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D76" s="10" t="s">
+      <c r="D76" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E76" s="18" t="s">
+      <c r="E76" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F76" s="12"/>
+      <c r="F76" s="14"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="18"/>
-      <c r="F77" s="12"/>
+      <c r="A77" s="13"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="16"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="10" t="s">
+      <c r="A78" s="13"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E78" s="18"/>
-      <c r="F78" s="12"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="14"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="12"/>
+      <c r="A79" s="13"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="14"/>
     </row>
     <row r="80" spans="1:6" ht="84" x14ac:dyDescent="0.25">
-      <c r="A80" s="12">
+      <c r="A80" s="13">
         <v>18</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D80" s="10" t="s">
+      <c r="D80" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E80" s="18" t="s">
+      <c r="E80" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F80" s="12"/>
+      <c r="F80" s="14"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="12"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="12"/>
+      <c r="A81" s="13"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="14"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="12"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="18"/>
-      <c r="F82" s="12"/>
+      <c r="A82" s="13"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="14"/>
     </row>
     <row r="83" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A83" s="12"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="10" t="s">
+      <c r="A83" s="13"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E83" s="18"/>
-      <c r="F83" s="12"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="14"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="12"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="12"/>
+      <c r="A84" s="13"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="14"/>
     </row>
     <row r="85" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A85" s="12">
+      <c r="A85" s="13">
         <v>19</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B85" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D85" s="10" t="s">
+      <c r="D85" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E85" s="18" t="s">
+      <c r="E85" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="18"/>
+      <c r="A86" s="13"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="13"/>
     </row>
     <row r="87" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A87" s="12"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="7"/>
-      <c r="D87" s="10" t="s">
+      <c r="A87" s="13"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E87" s="18"/>
+      <c r="E87" s="13"/>
     </row>
     <row r="88" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="13" t="s">
+      <c r="A88" s="13"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E88" s="18"/>
+      <c r="E88" s="13"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="7"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="18"/>
+      <c r="A89" s="13"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="16"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="13"/>
     </row>
     <row r="90" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="10" t="s">
+      <c r="A90" s="13"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="16"/>
+      <c r="D90" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E90" s="18"/>
+      <c r="E90" s="13"/>
     </row>
     <row r="91" spans="1:6" ht="48" x14ac:dyDescent="0.25">
       <c r="A91" s="11">
         <v>20</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B91" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C91" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="D91" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E91" s="19" t="s">
+      <c r="E91" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="12">
+      <c r="A92" s="13">
         <v>21</v>
       </c>
-      <c r="B92" s="12" t="s">
+      <c r="B92" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C92" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D92" s="14" t="s">
+      <c r="D92" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="E92" s="18" t="s">
+      <c r="E92" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="12"/>
-      <c r="B93" s="12"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="14"/>
-      <c r="E93" s="18"/>
+      <c r="A93" s="13"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="16"/>
+      <c r="D93" s="17"/>
+      <c r="E93" s="13"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="12"/>
-      <c r="B94" s="12"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="18"/>
+      <c r="A94" s="13"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="13"/>
     </row>
     <row r="95" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A95" s="12">
+      <c r="A95" s="13">
         <v>22</v>
       </c>
-      <c r="B95" s="12" t="s">
+      <c r="B95" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C95" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D95" s="10" t="s">
+      <c r="D95" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E95" s="18" t="s">
+      <c r="E95" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="18"/>
+      <c r="A96" s="13"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="13"/>
     </row>
     <row r="97" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="10" t="s">
+      <c r="A97" s="13"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="16"/>
+      <c r="D97" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E97" s="18"/>
+      <c r="E97" s="13"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="18"/>
+      <c r="A98" s="13"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="13"/>
     </row>
     <row r="99" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="10" t="s">
+      <c r="A99" s="13"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="16"/>
+      <c r="D99" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E99" s="18"/>
+      <c r="E99" s="13"/>
     </row>
     <row r="100" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
-      <c r="B100" s="12"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="10" t="s">
+      <c r="A100" s="13"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E100" s="18"/>
+      <c r="E100" s="13"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
-      <c r="B101" s="12"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="18"/>
+      <c r="A101" s="13"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="16"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="13"/>
     </row>
     <row r="102" spans="1:6" ht="84" x14ac:dyDescent="0.25">
-      <c r="A102" s="12"/>
-      <c r="B102" s="12"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="10" t="s">
+      <c r="A102" s="13"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E102" s="18"/>
+      <c r="E102" s="13"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
-      <c r="C103" s="7"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="18"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="16"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="13"/>
     </row>
     <row r="104" spans="1:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="A104" s="12"/>
-      <c r="B104" s="12"/>
-      <c r="C104" s="7"/>
-      <c r="D104" s="10" t="s">
+      <c r="A104" s="13"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E104" s="18"/>
+      <c r="E104" s="13"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="12"/>
-      <c r="B105" s="12"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="18"/>
+      <c r="A105" s="13"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="16"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="13"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="12"/>
-      <c r="B106" s="12"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="10"/>
-      <c r="E106" s="18"/>
+      <c r="A106" s="13"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="16"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="13"/>
     </row>
     <row r="107" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="11">
         <v>23</v>
       </c>
-      <c r="B107" s="11" t="s">
+      <c r="B107" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C107" s="4"/>
-      <c r="D107" s="10" t="s">
+      <c r="C107" s="3"/>
+      <c r="D107" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E107" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F107" s="17"/>
+      <c r="E107" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F107" s="10"/>
     </row>
     <row r="108" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A108" s="12">
+      <c r="A108" s="13">
         <v>24</v>
       </c>
-      <c r="B108" s="12" t="s">
+      <c r="B108" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C108" s="7"/>
-      <c r="D108" s="10" t="s">
+      <c r="C108" s="16"/>
+      <c r="D108" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E108" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F108" s="17"/>
+      <c r="E108" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F108" s="10"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="12"/>
-      <c r="B109" s="12"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="10"/>
-      <c r="E109" s="18"/>
-      <c r="F109" s="17"/>
+      <c r="A109" s="13"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="16"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="10"/>
     </row>
     <row r="110" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A110" s="12"/>
-      <c r="B110" s="12"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="10" t="s">
+      <c r="A110" s="13"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E110" s="18"/>
-      <c r="F110" s="17"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="10"/>
     </row>
     <row r="111" spans="1:6" ht="48" x14ac:dyDescent="0.25">
-      <c r="A111" s="12"/>
-      <c r="B111" s="12"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="13" t="s">
+      <c r="A111" s="13"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="16"/>
+      <c r="D111" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E111" s="18"/>
-      <c r="F111" s="17"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="10"/>
     </row>
     <row r="112" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A112" s="12">
+      <c r="A112" s="13">
         <v>25</v>
       </c>
-      <c r="B112" s="12" t="s">
+      <c r="B112" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C112" s="7"/>
-      <c r="D112" s="10" t="s">
+      <c r="C112" s="16"/>
+      <c r="D112" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E112" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F112" s="17"/>
+      <c r="E112" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F112" s="10"/>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A113" s="12"/>
-      <c r="B113" s="12"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="10"/>
-      <c r="E113" s="18"/>
-      <c r="F113" s="17"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="16"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="10"/>
     </row>
     <row r="114" spans="1:12" ht="24" x14ac:dyDescent="0.25">
-      <c r="A114" s="12"/>
-      <c r="B114" s="12"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="10" t="s">
+      <c r="A114" s="13"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="16"/>
+      <c r="D114" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E114" s="18"/>
-      <c r="F114" s="17"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="10"/>
     </row>
     <row r="115" spans="1:12" ht="48" x14ac:dyDescent="0.25">
-      <c r="A115" s="12"/>
-      <c r="B115" s="12"/>
-      <c r="C115" s="7"/>
-      <c r="D115" s="13" t="s">
+      <c r="A115" s="13"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="16"/>
+      <c r="D115" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E115" s="18"/>
-      <c r="F115" s="17"/>
-      <c r="I115" s="16"/>
-      <c r="J115" s="16"/>
-      <c r="K115" s="16"/>
-      <c r="L115" s="16"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="10"/>
+      <c r="I115" s="9"/>
+      <c r="J115" s="9"/>
+      <c r="K115" s="9"/>
+      <c r="L115" s="9"/>
     </row>
     <row r="116" spans="1:12" ht="84" x14ac:dyDescent="0.25">
       <c r="A116" s="11">
         <v>26</v>
       </c>
-      <c r="B116" s="11" t="s">
+      <c r="B116" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C116" s="4"/>
-      <c r="D116" s="10" t="s">
+      <c r="C116" s="3"/>
+      <c r="D116" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E116" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F116" s="17"/>
-      <c r="I116" s="16"/>
-      <c r="J116" s="5"/>
-      <c r="K116" s="16"/>
-      <c r="L116" s="16"/>
+      <c r="E116" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F116" s="10"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="9"/>
+      <c r="L116" s="9"/>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="11">
         <v>27</v>
       </c>
-      <c r="B117" s="11"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="10"/>
-      <c r="E117" s="20"/>
-      <c r="F117" s="17"/>
-      <c r="I117" s="16"/>
-      <c r="J117" s="5"/>
-      <c r="K117" s="16"/>
-      <c r="L117" s="16"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="10"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="9"/>
+      <c r="L117" s="9"/>
     </row>
     <row r="118" spans="1:12" ht="36" x14ac:dyDescent="0.25">
-      <c r="A118" s="12">
+      <c r="A118" s="13">
         <v>28</v>
       </c>
       <c r="B118" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C118" s="7" t="s">
+      <c r="C118" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="D118" s="10" t="s">
+      <c r="D118" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E118" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F118" s="17"/>
-      <c r="I118" s="16"/>
-      <c r="J118" s="16"/>
-      <c r="K118" s="16"/>
-      <c r="L118" s="16"/>
+      <c r="E118" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F118" s="10"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="9"/>
+      <c r="K118" s="9"/>
+      <c r="L118" s="9"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A119" s="12"/>
+      <c r="A119" s="13"/>
       <c r="B119" s="15"/>
-      <c r="C119" s="7"/>
-      <c r="D119" s="10"/>
-      <c r="E119" s="18"/>
-      <c r="F119" s="17"/>
-      <c r="I119" s="16"/>
-      <c r="J119" s="16"/>
-      <c r="K119" s="16"/>
-      <c r="L119" s="16"/>
+      <c r="C119" s="16"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="10"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="9"/>
+      <c r="K119" s="9"/>
+      <c r="L119" s="9"/>
     </row>
     <row r="120" spans="1:12" ht="36" x14ac:dyDescent="0.25">
-      <c r="A120" s="12"/>
+      <c r="A120" s="13"/>
       <c r="B120" s="15"/>
-      <c r="C120" s="7"/>
-      <c r="D120" s="10" t="s">
+      <c r="C120" s="16"/>
+      <c r="D120" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E120" s="18"/>
-      <c r="F120" s="17"/>
-      <c r="I120" s="16"/>
-      <c r="J120" s="16"/>
-      <c r="K120" s="16"/>
-      <c r="L120" s="16"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="10"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="9"/>
+      <c r="K120" s="9"/>
+      <c r="L120" s="9"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A121" s="12"/>
+      <c r="A121" s="13"/>
       <c r="B121" s="15"/>
-      <c r="C121" s="7"/>
-      <c r="D121" s="10"/>
-      <c r="E121" s="18"/>
-      <c r="F121" s="17"/>
-      <c r="I121" s="16"/>
-      <c r="J121" s="16"/>
-      <c r="K121" s="16"/>
-      <c r="L121" s="16"/>
+      <c r="C121" s="16"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="10"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="9"/>
+      <c r="K121" s="9"/>
+      <c r="L121" s="9"/>
     </row>
     <row r="122" spans="1:12" ht="36" x14ac:dyDescent="0.25">
-      <c r="A122" s="12"/>
+      <c r="A122" s="13"/>
       <c r="B122" s="15"/>
-      <c r="C122" s="7"/>
-      <c r="D122" s="10" t="s">
+      <c r="C122" s="16"/>
+      <c r="D122" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E122" s="18"/>
-      <c r="F122" s="17"/>
-      <c r="I122" s="16"/>
-      <c r="J122" s="16"/>
-      <c r="K122" s="16"/>
-      <c r="L122" s="16"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="10"/>
+      <c r="I122" s="9"/>
+      <c r="J122" s="9"/>
+      <c r="K122" s="9"/>
+      <c r="L122" s="9"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A123" s="12"/>
+      <c r="A123" s="13"/>
       <c r="B123" s="15"/>
-      <c r="C123" s="7"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="18"/>
-      <c r="F123" s="17"/>
+      <c r="C123" s="16"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="10"/>
     </row>
     <row r="124" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A124" s="11">
         <v>29</v>
       </c>
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C124" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D124" s="10" t="s">
+      <c r="D124" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E124" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F124" s="17"/>
+      <c r="E124" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F124" s="10"/>
     </row>
     <row r="125" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A125" s="11">
         <v>30</v>
       </c>
-      <c r="B125" s="11" t="s">
+      <c r="B125" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C125" s="4" t="s">
+      <c r="C125" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D125" s="10" t="s">
+      <c r="D125" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E125" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F125" s="17"/>
+      <c r="E125" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F125" s="10"/>
     </row>
     <row r="126" spans="1:12" ht="36" x14ac:dyDescent="0.25">
       <c r="A126" s="11">
         <v>31</v>
       </c>
-      <c r="B126" s="11" t="s">
+      <c r="B126" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C126" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D126" s="10" t="s">
+      <c r="D126" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E126" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F126" s="17"/>
+      <c r="E126" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F126" s="10"/>
     </row>
     <row r="127" spans="1:12" ht="72" x14ac:dyDescent="0.25">
       <c r="A127" s="11">
         <v>32</v>
       </c>
-      <c r="B127" s="11" t="s">
+      <c r="B127" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C127" s="4"/>
-      <c r="D127" s="10" t="s">
+      <c r="C127" s="3"/>
+      <c r="D127" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E127" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F127" s="17"/>
+      <c r="E127" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F127" s="10"/>
     </row>
     <row r="128" spans="1:12" ht="72" x14ac:dyDescent="0.25">
       <c r="A128" s="11">
         <v>33</v>
       </c>
-      <c r="B128" s="11" t="s">
+      <c r="B128" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C128" s="4"/>
-      <c r="D128" s="10" t="s">
+      <c r="C128" s="3"/>
+      <c r="D128" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E128" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F128" s="17"/>
+      <c r="E128" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F128" s="10"/>
     </row>
     <row r="129" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A129" s="11">
         <v>34</v>
       </c>
-      <c r="B129" s="11" t="s">
+      <c r="B129" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C129" s="4"/>
-      <c r="D129" s="10" t="s">
+      <c r="C129" s="3"/>
+      <c r="D129" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E129" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F129" s="17"/>
+      <c r="E129" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F129" s="10"/>
     </row>
     <row r="130" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A130" s="12">
+      <c r="A130" s="13">
         <v>35</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B130" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C130" s="7"/>
-      <c r="D130" s="10" t="s">
+      <c r="C130" s="16"/>
+      <c r="D130" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E130" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F130" s="17"/>
+      <c r="E130" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F130" s="10"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="12"/>
-      <c r="B131" s="12"/>
-      <c r="C131" s="7"/>
-      <c r="D131" s="10" t="s">
+      <c r="A131" s="13"/>
+      <c r="B131" s="14"/>
+      <c r="C131" s="16"/>
+      <c r="D131" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="E131" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F131" s="17"/>
+      <c r="E131" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F131" s="10"/>
     </row>
     <row r="132" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A132" s="11">
         <v>36</v>
       </c>
-      <c r="B132" s="11" t="s">
+      <c r="B132" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C132" s="4"/>
-      <c r="D132" s="10" t="s">
+      <c r="C132" s="3"/>
+      <c r="D132" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E132" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F132" s="17"/>
+      <c r="E132" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F132" s="10"/>
     </row>
     <row r="133" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A133" s="11">
         <v>37</v>
       </c>
-      <c r="B133" s="11" t="s">
+      <c r="B133" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C133" s="4"/>
-      <c r="D133" s="10" t="s">
+      <c r="C133" s="3"/>
+      <c r="D133" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E133" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F133" s="17"/>
+      <c r="E133" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F133" s="10"/>
     </row>
     <row r="134" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A134" s="11">
         <v>38</v>
       </c>
-      <c r="B134" s="11" t="s">
+      <c r="B134" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C134" s="4"/>
-      <c r="D134" s="10" t="s">
+      <c r="C134" s="3"/>
+      <c r="D134" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E134" s="20" t="s">
+      <c r="E134" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F134" s="17"/>
+      <c r="F134" s="10"/>
     </row>
     <row r="135" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="12">
+      <c r="A135" s="13">
         <v>39</v>
       </c>
       <c r="B135" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C135" s="7"/>
-      <c r="D135" s="14" t="s">
+      <c r="C135" s="16"/>
+      <c r="D135" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E135" s="18" t="s">
+      <c r="E135" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F135" s="12"/>
+      <c r="F135" s="14"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="12"/>
+      <c r="A136" s="13"/>
       <c r="B136" s="15"/>
-      <c r="C136" s="7"/>
-      <c r="D136" s="14"/>
-      <c r="E136" s="18"/>
-      <c r="F136" s="12"/>
+      <c r="C136" s="16"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="14"/>
     </row>
     <row r="137" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A137" s="11">
         <v>40</v>
       </c>
-      <c r="B137" s="11" t="s">
+      <c r="B137" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C137" s="4"/>
-      <c r="D137" s="10" t="s">
+      <c r="C137" s="3"/>
+      <c r="D137" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E137" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F137" s="11"/>
+      <c r="E137" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F137" s="7"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" s="11"/>
-      <c r="B138" s="11"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="10"/>
-      <c r="E138" s="11"/>
-      <c r="F138" s="11"/>
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="6"/>
+      <c r="E138" s="7"/>
+      <c r="F138" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="111">
+  <mergeCells count="112">
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="E15:E21"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="E33:E39"/>
+    <mergeCell ref="F33:F39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="E44:E50"/>
+    <mergeCell ref="F44:F50"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="B51:B58"/>
+    <mergeCell ref="C51:C58"/>
+    <mergeCell ref="E51:E58"/>
+    <mergeCell ref="F51:F58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="A62:A69"/>
+    <mergeCell ref="B62:B69"/>
+    <mergeCell ref="C62:C69"/>
+    <mergeCell ref="E62:E69"/>
+    <mergeCell ref="F62:F69"/>
+    <mergeCell ref="F80:F84"/>
+    <mergeCell ref="A85:A90"/>
+    <mergeCell ref="B85:B90"/>
+    <mergeCell ref="C85:C90"/>
+    <mergeCell ref="E85:E90"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="C72:C75"/>
+    <mergeCell ref="E72:E75"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="A76:A79"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="C76:C79"/>
+    <mergeCell ref="E76:E79"/>
+    <mergeCell ref="F76:F79"/>
+    <mergeCell ref="C92:C94"/>
+    <mergeCell ref="D92:D94"/>
+    <mergeCell ref="E92:E94"/>
+    <mergeCell ref="A95:A106"/>
+    <mergeCell ref="B95:B106"/>
+    <mergeCell ref="C95:C106"/>
+    <mergeCell ref="E95:E106"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="E80:E84"/>
     <mergeCell ref="E108:E111"/>
     <mergeCell ref="E112:E115"/>
     <mergeCell ref="E118:E123"/>
@@ -2499,95 +2651,9 @@
     <mergeCell ref="C112:C115"/>
     <mergeCell ref="A92:A94"/>
     <mergeCell ref="B92:B94"/>
-    <mergeCell ref="C92:C94"/>
-    <mergeCell ref="D92:D94"/>
-    <mergeCell ref="E92:E94"/>
-    <mergeCell ref="A95:A106"/>
-    <mergeCell ref="B95:B106"/>
-    <mergeCell ref="C95:C106"/>
-    <mergeCell ref="E95:E106"/>
-    <mergeCell ref="A80:A84"/>
-    <mergeCell ref="B80:B84"/>
-    <mergeCell ref="C80:C84"/>
-    <mergeCell ref="E80:E84"/>
-    <mergeCell ref="F80:F84"/>
-    <mergeCell ref="A85:A90"/>
-    <mergeCell ref="B85:B90"/>
-    <mergeCell ref="C85:C90"/>
-    <mergeCell ref="E85:E90"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="C72:C75"/>
-    <mergeCell ref="E72:E75"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="A76:A79"/>
-    <mergeCell ref="B76:B79"/>
-    <mergeCell ref="C76:C79"/>
-    <mergeCell ref="E76:E79"/>
-    <mergeCell ref="F76:F79"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="A62:A69"/>
-    <mergeCell ref="B62:B69"/>
-    <mergeCell ref="C62:C69"/>
-    <mergeCell ref="E62:E69"/>
-    <mergeCell ref="F62:F69"/>
-    <mergeCell ref="A51:A58"/>
-    <mergeCell ref="B51:B58"/>
-    <mergeCell ref="C51:C58"/>
-    <mergeCell ref="E51:E58"/>
-    <mergeCell ref="F51:F58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="F40:F43"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="E44:E50"/>
-    <mergeCell ref="F44:F50"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="E33:E39"/>
-    <mergeCell ref="F33:F39"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="A15:A21"/>
-    <mergeCell ref="B15:B21"/>
-    <mergeCell ref="C15:C21"/>
-    <mergeCell ref="E15:E21"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>